<commit_message>
Moved Project & Portfolio files to "logs" folder. Updated Time Estimation Worksheet Added New Burn-Up List Added New Project & Portfolio assignment
</commit_message>
<xml_diff>
--- a/logs/JacksonAaron_Time Estimation.xlsx
+++ b/logs/JacksonAaron_Time Estimation.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="6020" yWindow="1120" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>JacksonAaron</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>Week 3</t>
-  </si>
-  <si>
-    <t>Week 4</t>
   </si>
   <si>
     <t>Career Module</t>
@@ -545,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1017"/>
+  <dimension ref="A1:E1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -802,40 +799,46 @@
     <row r="21" spans="1:5" ht="24" customHeight="1">
       <c r="A21" s="13"/>
       <c r="B21" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" s="9">
         <v>60</v>
       </c>
-      <c r="D21" s="9"/>
+      <c r="D21" s="9">
+        <v>60</v>
+      </c>
       <c r="E21" s="11">
         <f>C21 -D21</f>
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="24" customHeight="1">
       <c r="A22" s="13"/>
       <c r="B22" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="9">
         <v>60</v>
       </c>
-      <c r="D22" s="9"/>
+      <c r="D22" s="9">
+        <v>45</v>
+      </c>
       <c r="E22" s="11">
         <f>C22-D22</f>
-        <v>60</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="24" customHeight="1">
       <c r="A23" s="13"/>
       <c r="B23" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="9">
         <v>60</v>
       </c>
-      <c r="D23" s="9"/>
+      <c r="D23" s="9">
+        <v>0</v>
+      </c>
       <c r="E23" s="11">
         <f>C23-D23</f>
         <v>60</v>
@@ -844,38 +847,37 @@
     <row r="24" spans="1:5" ht="24" customHeight="1">
       <c r="A24" s="13"/>
       <c r="B24" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" s="9">
         <v>10</v>
       </c>
-      <c r="D24" s="9"/>
+      <c r="D24" s="9">
+        <v>5</v>
+      </c>
       <c r="E24" s="11">
         <f>C24-D24</f>
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="24" customHeight="1">
       <c r="A25" s="13"/>
       <c r="B25" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" s="9">
         <v>25</v>
       </c>
-      <c r="D25" s="9"/>
+      <c r="D25" s="9">
+        <v>20</v>
+      </c>
       <c r="E25" s="11">
         <f>C25-D25</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="66" customHeight="1">
-      <c r="A26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="12">
+      <c r="A26" s="12"/>
       <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:5" ht="12">
@@ -4837,10 +4839,6 @@
     <row r="1016" spans="1:5" ht="12">
       <c r="A1016" s="12"/>
       <c r="E1016" s="7"/>
-    </row>
-    <row r="1017" spans="1:5" ht="12">
-      <c r="A1017" s="12"/>
-      <c r="E1017" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>